<commit_message>
Change API to obtain specific nutrient instead of calories only
</commit_message>
<xml_diff>
--- a/food-dataset.xlsx
+++ b/food-dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tangj\OneDrive\Desktop\4rd Year 2nd Sem\FYP 1\Jin Hang FYP codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D910F9-BDEF-4E7E-BFC1-5415F16783B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81D06E3-72E3-4367-823A-2990AFBE475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB2E8D99-9522-F742-92B6-897572B481CE}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{FB2E8D99-9522-F742-92B6-897572B481CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <r>
       <t xml:space="preserve">Bil.
@@ -69,10 +69,6 @@
       </rPr>
       <t>Household measurement</t>
     </r>
-  </si>
-  <si>
-    <t>Protein 
-(g)</t>
   </si>
   <si>
     <r>
@@ -348,30 +344,6 @@
     </r>
   </si>
   <si>
-    <t>CHO (carbohydrate)
-(g)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t xml:space="preserve">Fat
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ArialMT"/>
-      </rPr>
-      <t>(g)</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <i/>
@@ -450,6 +422,18 @@
   </si>
   <si>
     <t>White Bread</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t>Carbohydrate</t>
+  </si>
+  <si>
+    <t>Protein</t>
   </si>
 </sst>
 </file>
@@ -916,7 +900,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.08984375" defaultRowHeight="15"/>
@@ -931,43 +915,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6">
@@ -975,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6">
         <v>47</v>
@@ -1019,10 +1003,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6">
         <v>40</v>
@@ -1063,10 +1047,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6">
         <v>50</v>
@@ -1107,10 +1091,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6">
         <v>21</v>
@@ -1143,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45.6">
@@ -1151,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="6">
         <v>29</v>
@@ -1187,7 +1171,7 @@
         <v>0.5</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="45.6">
@@ -1195,10 +1179,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="6">
         <v>30</v>
@@ -1231,7 +1215,7 @@
         <v>0.6</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.6">
@@ -1239,10 +1223,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="6">
         <v>92</v>
@@ -1283,10 +1267,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="6">
         <v>115</v>
@@ -1327,10 +1311,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="6">
         <v>62</v>
@@ -1371,10 +1355,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6">
         <v>84</v>
@@ -1414,8 +1398,15 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="6">
+        <v>50</v>
+      </c>
+      <c r="E12" s="6">
+        <v>100</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -5937,6 +5928,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>